<commit_message>
fix missing session info; close #1144
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/cards/Card-A4.xlsx
+++ b/owlcms/src/main/resources/templates/cards/Card-A4.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC35993-B287-43EC-A960-03E6BD1DF9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DF937E-9732-4890-B65F-9869D96F4204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="3255" windowWidth="19590" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A:$I</definedName>
+  </definedNames>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -59,26 +62,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{DD5D7428-31E2-4FD5-9552-E92A8463D510}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color rgb="FF000000"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-          </rPr>
-          <t>jx:area(
-  lastCell="I24"
-)
-jx:each(
-  items="athletes"
-  var="athlete"
-  lastCell="I24"
-)</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -634,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -725,9 +708,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1171,10 +1151,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,14 +1163,14 @@
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="4.7109375" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -1212,67 +1192,67 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="F2" s="36" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="F2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="38"/>
-      <c r="I2" s="39"/>
-    </row>
-    <row r="3" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="37"/>
+      <c r="I2" s="38"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
-    </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="44"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="55" t="s">
+      <c r="G4" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="56"/>
-      <c r="I4" s="57"/>
-    </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="H4" s="55"/>
+      <c r="I4" s="56"/>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="52"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="51"/>
       <c r="H5" s="10" t="s">
         <v>22</v>
       </c>
@@ -1280,11 +1260,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="54"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="27" t="s">
         <v>23</v>
       </c>
@@ -1292,10 +1272,10 @@
         <v>24</v>
       </c>
       <c r="E6" s="26"/>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="54"/>
+      <c r="G6" s="53"/>
       <c r="H6" s="11" t="s">
         <v>20</v>
       </c>
@@ -1303,7 +1283,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1318,57 +1298,56 @@
         <v>26</v>
       </c>
       <c r="G7" s="12"/>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="50"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="24"/>
       <c r="D8" s="16"/>
-      <c r="F8" s="58" t="s">
+      <c r="F8" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="59"/>
+      <c r="G8" s="58"/>
       <c r="H8" s="28"/>
       <c r="I8" s="25"/>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
+    </row>
+    <row r="9" spans="1:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
-      <c r="F9" s="60" t="s">
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="47"/>
+      <c r="F9" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="62"/>
-    </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="63">
-        <v>1</v>
-      </c>
-      <c r="B10" s="64"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="61"/>
+    </row>
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="62">
+        <v>1</v>
+      </c>
+      <c r="B10" s="63"/>
       <c r="C10" s="13">
         <v>2</v>
       </c>
       <c r="D10" s="14">
         <v>3</v>
       </c>
-      <c r="F10" s="63">
-        <v>1</v>
-      </c>
-      <c r="G10" s="64"/>
+      <c r="F10" s="62">
+        <v>1</v>
+      </c>
+      <c r="G10" s="63"/>
       <c r="H10" s="13">
         <v>2</v>
       </c>
@@ -1376,17 +1355,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
-      <c r="B11" s="66"/>
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="64"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="29" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
       <c r="H11" s="29" t="s">
         <v>16</v>
       </c>
@@ -1394,17 +1373,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
-      <c r="B12" s="68"/>
+    <row r="12" spans="1:9" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="66"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="31"/>
       <c r="D12" s="32"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="68"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="31"/>
       <c r="I12" s="32"/>
     </row>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1426,7 +1405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -1436,7 +1415,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>1</v>
       </c>
@@ -1458,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="29.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="5"/>
@@ -1595,16 +1574,6 @@
       <c r="G24" s="18"/>
       <c r="H24" s="17"/>
       <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>